<commit_message>
the test case document was modified according to the indications
</commit_message>
<xml_diff>
--- a/DesignAndExecution/Casos de pruebas.xlsx
+++ b/DesignAndExecution/Casos de pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\OneDrive\Escritorio\Punto Singular\Proyecto Plan de Pruebas\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA43E7B-107F-42C4-999A-CF6619C54D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB8EC14-193A-46A3-B0F3-A4DE4FC2268F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="116">
   <si>
     <t>Identificador</t>
   </si>
@@ -111,10 +111,6 @@
     <t>CP9</t>
   </si>
   <si>
-    <t>1. Ir a la opción de Subir Imagen y hacer clic.
-2. Llena los datos necesarios.                              3. Subir imagen                                         4. Click en el botón de continuar.        5. Clic en el botón de finalizar</t>
-  </si>
-  <si>
     <t>1. Ir a la opción de Subir Imagen y hacer clic (url** /pet/{petId}/uploadImage).
 2. Llena el identificador con diferentes caracteres (12345).                                   3. Subir imagen                                        4. Click en el botón de continuar.        5. Clic en el botón de finalizar</t>
   </si>
@@ -168,20 +164,12 @@
     <t>CP14</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/{petId} usando el método GET
-2. El petId solo debe ser un número entero                                                         3. Click en el botón de continuar búsqueda.                                                        </t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/findByStatus
 2. findByStatus: estado de la mascota (available - pending - sold) - string. 3. Click en el botón de continuar búsqueda.                                                     </t>
   </si>
   <si>
     <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/findByStatus
 2. findByStatus: estado de la mascota (available - pending - sold) - string. Mandando un valor incorrecto ya sea con números o un valor vacío.            3. Click en el botón de continuar búsqueda.                                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/{petId} usando el método GET
-2. El campo pedId se llenará con el dato: 'vacío' o 'caracteres'                                                         3. Click en el botón de continuar búsqueda.                                                        </t>
   </si>
   <si>
     <t>CP15</t>
@@ -221,10 +209,6 @@
   </si>
   <si>
     <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clicurl** /pet/{petId} usando el método Metodo DELETE
-2. Se seleccionará la mascota la cual se quiere eliminar usando el petId del mismo (número entero).                                                        3. Click en el botón de Eliminar mascota.                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clicurl** /pet/{petId} usando el método Metodo DELETE
 2. Se seleccionará la mascota la cual se quiere eliminar usando el petId del mismo (usando una cadena ya se por medio del nombre de la mascota o no seleccionar laguna mascota).                                                        3. Click en el botón de Eliminar mascota.                                                        </t>
   </si>
   <si>
@@ -258,12 +242,6 @@
     <t>3. Si petId no es valido se debe mostrar status code 400 Pet not found, este campo se tomará como inválido y se cancelará la búsqueda.</t>
   </si>
   <si>
-    <t>3. Si la petición es correcta se debe mostrar status code 200 con la mascota buscada, este campo se tomará como válido y procederá en la búsqueda</t>
-  </si>
-  <si>
-    <t>3. Si los valores del ID son solo números enteros, este campo se tomará como válido y procederá en la búsqueda</t>
-  </si>
-  <si>
     <t xml:space="preserve">3. Si la petición es correcta se debe mostrar status code 200 con un listado de las mascotas que coinciden con el estado </t>
   </si>
   <si>
@@ -295,6 +273,143 @@
   </si>
   <si>
     <t>5. Finalizair el proceso y corroborar que se realizó correctamente mandando status code 200 OK.</t>
+  </si>
+  <si>
+    <t>1. Ir a la opción de Subir Imagen y hacer clic (url** /pet/{petId}/uploadImage)..
+2. Llena el identificador con diferentes caracteres (mascota12333).                  3. Subir imagen                                            4. Click en el botón de continuar.           5. Clic en el botón de finalizar</t>
+  </si>
+  <si>
+    <t>Validar que los datos de la mascota para subir su imagen sean correctos. El petId tendrá caracteres, no depe pasar de 15 caracteres, tiene que ser  String y numérico</t>
+  </si>
+  <si>
+    <t>Validar que los datos de la mascota para subir su imagen sean correctos. El petId estará vación, sin recibir ningún valor</t>
+  </si>
+  <si>
+    <t>CP20</t>
+  </si>
+  <si>
+    <t>CP21</t>
+  </si>
+  <si>
+    <t>CP22</t>
+  </si>
+  <si>
+    <t>No sobir ninguna imagen, quedando vació en el apartado de subir imagen.</t>
+  </si>
+  <si>
+    <t>1. Ir a la opción de Subir Imagen y hacer clic(url** /pet/{petId}/uploadImage)..
+2. Llena los datos necesarios.                              3. Subir imagen                                         4. Click en el botón de continuar.        5. Clic en el botón de finalizar</t>
+  </si>
+  <si>
+    <t>1. Ir a la opción de Subir Imagen y hacer clic(url** /pet/{petId}/uploadImage)..
+2. Llena los datos necesarios.                              3. No subir imagen                                         4. Click en el botón de continuar.        5. Clic en el botón de finalizar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Debe mostrar status code 400 Pet not found. Falta subir algún archivo en formato de imagen </t>
+  </si>
+  <si>
+    <t>CP23</t>
+  </si>
+  <si>
+    <t>CP24</t>
+  </si>
+  <si>
+    <t>CP25</t>
+  </si>
+  <si>
+    <t>CP26</t>
+  </si>
+  <si>
+    <t>CP27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clicurl** /pet/{petId} usando el  Metodo DELETE
+2. Se seleccionará la mascota la cual se quiere eliminar usando el petId del mismo (número entero).                                                        3. Click en el botón de Eliminar mascota.                                                        </t>
+  </si>
+  <si>
+    <t>Como administrador quiero eliminar una mascota para depurar la información, no se seleccionará ningun indentificador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clicurl** /pet/{petId} usando el método Metodo DELETE
+2. No se seleccionará alguna mascota                                                      3. Click en el botón de Eliminar mascota.                                                        </t>
+  </si>
+  <si>
+    <t>3. Debe mostrar status code 400 Pet not found.</t>
+  </si>
+  <si>
+    <t>1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet.
+2. No llenar datos, dejándolos de manera vacía                                                           3. No subir ninguna imagen                                 4.Poner el status de la mascota                                     5. Click en el botón de continuar.        6. Clic en el botón de finalizar</t>
+  </si>
+  <si>
+    <t>1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet.
+2. No ingresar datos                                    3. No subir imágen                                    4. Click en el botón de continuar.           5. Clic en el botón de finalizar</t>
+  </si>
+  <si>
+    <t>1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet.
+2. No ingresar datos                                    3. Subir imagen (URL) correctamente                                    4. Click en el botón de continuar.           5. Clic en el botón de finalizar</t>
+  </si>
+  <si>
+    <t>1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet.
+2. Llena los datos necesarios.                 3. Subir imagen (URL) incorrecta                                    4. Click en el botón de continuar.           5. Clic en el botón de finalizar</t>
+  </si>
+  <si>
+    <t>CP28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/{petId} usando el método Metodo POST
+2. Engresar en la URL un petId no existente con número enteros (12349883)                                                    3. Click en el botón de Actualizar mascota.                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clicurl** /pet/{petId} usando el método Metodo DELETE
+2. ingresar un identificador no existente en la URL petId usando números enteros (123987354)                                                      3. Click en el botón de Eliminar mascota.                                                        </t>
+  </si>
+  <si>
+    <t>CP29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/{petId} usando el método GET
+2. El campo pedId se llenará con el dato: 'vacío'                                               3. Click en el botón de continuar búsqueda.                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/{petId} usando el método GET
+2. El campo pedId se llenará con el dato: 'caracters' sin pasar los 10 caracteres                                                 3. Click en el botón de continuar búsqueda.                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/{petId} usando el método GET
+2. El petId solo debe ser un número entero                                                                       3. Filtrar la búsqueda por "disponibles"                                                         4. Click en el botón de continuar búsqueda.                                                        </t>
+  </si>
+  <si>
+    <t>4. Si los valores del ID son solo números enteros, este campo se tomará como válido y procederá en la búsqueda, debe mostrar status code 200</t>
+  </si>
+  <si>
+    <t>4. Si los valores del ID son solo números enteros, este campo se tomará como válido y procederá en la búsqueda, debe mostrar status code 201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/{petId} usando el método GET
+2. El petId solo debe ser un número entero                                                                       3. Filtrar la búsqueda por "pendientes"                                                         4. Click en el botón de continuar búsqueda.                                                        </t>
+  </si>
+  <si>
+    <t>4. Si los valores del ID son solo números enteros, este campo se tomará como válido y procederá en la búsqueda, debe mostrar status code 202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/{petId} usando el método GET
+2. El petId solo debe ser un número entero                                                                       3. Filtrar la búsqueda por "vendidos"                                                         4. Click en el botón de continuar búsqueda.                                                        </t>
+  </si>
+  <si>
+    <t>3. Se debe mostrar status code 400 Pet not found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la opción de Agregar una mascota a la tienda y hacer clic url** /pet/{petId} usando el método GET
+2. El campo pedId se pondrá un identificador no existente, ingresando números aleatorios no más de ocho caracteres usandolo en cualquier de los tres filtros.                                               3. Click en el botón de continuar búsqueda.                                                        </t>
+  </si>
+  <si>
+    <t>CP30</t>
+  </si>
+  <si>
+    <t>CP31</t>
+  </si>
+  <si>
+    <t>CP32</t>
   </si>
 </sst>
 </file>
@@ -630,10 +745,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB1002"/>
+  <dimension ref="A1:AB1012"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -796,19 +911,19 @@
         <v>11</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -842,19 +957,19 @@
         <v>19</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -876,7 +991,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="118.8" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
       <c r="A7" s="1"/>
       <c r="B7" s="10" t="s">
         <v>13</v>
@@ -885,22 +1000,22 @@
         <v>10</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -922,7 +1037,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
       <c r="A8" s="1"/>
       <c r="B8" s="10" t="s">
         <v>15</v>
@@ -931,22 +1046,22 @@
         <v>10</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -968,16 +1083,32 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
       <c r="A9" s="1"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="B9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1001,28 +1132,28 @@
     <row r="10" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
       <c r="A10" s="1"/>
       <c r="B10" s="10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1047,28 +1178,28 @@
     <row r="11" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
       <c r="A11" s="1"/>
       <c r="B11" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1120,31 +1251,31 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="198" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
       <c r="A13" s="1"/>
       <c r="B13" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1166,31 +1297,31 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="217.8" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
       <c r="A14" s="1"/>
       <c r="B14" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1212,31 +1343,31 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" ht="158.4" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
       <c r="A15" s="1"/>
       <c r="B15" s="10" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1258,31 +1389,31 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="217.8" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
       <c r="A16" s="1"/>
       <c r="B16" s="10" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1334,31 +1465,31 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
+    <row r="18" spans="1:28" ht="198" x14ac:dyDescent="0.7">
       <c r="A18" s="1"/>
       <c r="B18" s="10" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1380,31 +1511,31 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:28" ht="217.8" x14ac:dyDescent="0.7">
       <c r="A19" s="1"/>
       <c r="B19" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1426,16 +1557,32 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:28" ht="158.4" x14ac:dyDescent="0.7">
       <c r="A20" s="1"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="B20" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1456,31 +1603,31 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:28" ht="217.8" x14ac:dyDescent="0.7">
       <c r="A21" s="1"/>
       <c r="B21" s="10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1502,31 +1649,31 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
       <c r="A22" s="1"/>
       <c r="B22" s="10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1548,32 +1695,16 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
+    <row r="23" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
       <c r="A23" s="1"/>
-      <c r="B23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1594,16 +1725,32 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="24" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
       <c r="A24" s="1"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="B24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1624,31 +1771,31 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="198" x14ac:dyDescent="0.7">
+    <row r="25" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
       <c r="A25" s="1"/>
       <c r="B25" s="10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1670,32 +1817,16 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" ht="198" x14ac:dyDescent="0.7">
+    <row r="26" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
       <c r="A26" s="1"/>
-      <c r="B26" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1716,31 +1847,31 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" ht="217.8" x14ac:dyDescent="0.7">
+    <row r="27" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
       <c r="A27" s="1"/>
       <c r="B27" s="10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1762,16 +1893,32 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="28" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
       <c r="A28" s="1"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
+      <c r="B28" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1792,31 +1939,31 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
+    <row r="29" spans="1:28" ht="158.4" x14ac:dyDescent="0.7">
       <c r="A29" s="1"/>
       <c r="B29" s="10" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H29" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="10" t="s">
+      <c r="I29" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -1838,31 +1985,31 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" ht="237.6" x14ac:dyDescent="0.7">
+    <row r="30" spans="1:28" ht="138.6" x14ac:dyDescent="0.7">
       <c r="A30" s="1"/>
       <c r="B30" s="10" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D30" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="I30" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -1884,16 +2031,32 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="31" spans="1:28" ht="158.4" x14ac:dyDescent="0.7">
       <c r="A31" s="1"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
+      <c r="B31" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1914,16 +2077,32 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="32" spans="1:28" ht="198" x14ac:dyDescent="0.7">
       <c r="A32" s="1"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
+      <c r="B32" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1946,14 +2125,14 @@
     </row>
     <row r="33" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
       <c r="A33" s="1"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1974,16 +2153,32 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="34" spans="1:28" ht="198" x14ac:dyDescent="0.7">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="B34" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -2004,16 +2199,32 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="35" spans="1:28" ht="198" x14ac:dyDescent="0.7">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="B35" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -2034,16 +2245,32 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="36" spans="1:28" ht="217.8" x14ac:dyDescent="0.7">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="B36" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -2064,16 +2291,32 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="37" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="B37" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -2096,14 +2339,14 @@
     </row>
     <row r="38" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -2124,16 +2367,32 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="39" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="B39" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -2154,16 +2413,32 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="40" spans="1:28" ht="237.6" x14ac:dyDescent="0.7">
       <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="B40" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -2184,16 +2459,32 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="41" spans="1:28" ht="158.4" x14ac:dyDescent="0.7">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="B41" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -2214,16 +2505,32 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="42" spans="1:28" ht="178.2" x14ac:dyDescent="0.7">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="B42" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -2246,14 +2553,14 @@
     </row>
     <row r="43" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -31044,10 +31351,310 @@
       <c r="AA1002" s="1"/>
       <c r="AB1002" s="1"/>
     </row>
+    <row r="1003" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="2"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+      <c r="AA1003" s="1"/>
+      <c r="AB1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="2"/>
+      <c r="F1004" s="1"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+      <c r="S1004" s="1"/>
+      <c r="T1004" s="1"/>
+      <c r="U1004" s="1"/>
+      <c r="V1004" s="1"/>
+      <c r="W1004" s="1"/>
+      <c r="X1004" s="1"/>
+      <c r="Y1004" s="1"/>
+      <c r="Z1004" s="1"/>
+      <c r="AA1004" s="1"/>
+      <c r="AB1004" s="1"/>
+    </row>
+    <row r="1005" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="1"/>
+      <c r="E1005" s="2"/>
+      <c r="F1005" s="1"/>
+      <c r="G1005" s="1"/>
+      <c r="H1005" s="1"/>
+      <c r="I1005" s="1"/>
+      <c r="J1005" s="1"/>
+      <c r="K1005" s="1"/>
+      <c r="L1005" s="1"/>
+      <c r="M1005" s="1"/>
+      <c r="N1005" s="1"/>
+      <c r="O1005" s="1"/>
+      <c r="P1005" s="1"/>
+      <c r="Q1005" s="1"/>
+      <c r="R1005" s="1"/>
+      <c r="S1005" s="1"/>
+      <c r="T1005" s="1"/>
+      <c r="U1005" s="1"/>
+      <c r="V1005" s="1"/>
+      <c r="W1005" s="1"/>
+      <c r="X1005" s="1"/>
+      <c r="Y1005" s="1"/>
+      <c r="Z1005" s="1"/>
+      <c r="AA1005" s="1"/>
+      <c r="AB1005" s="1"/>
+    </row>
+    <row r="1006" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="1"/>
+      <c r="E1006" s="2"/>
+      <c r="F1006" s="1"/>
+      <c r="G1006" s="1"/>
+      <c r="H1006" s="1"/>
+      <c r="I1006" s="1"/>
+      <c r="J1006" s="1"/>
+      <c r="K1006" s="1"/>
+      <c r="L1006" s="1"/>
+      <c r="M1006" s="1"/>
+      <c r="N1006" s="1"/>
+      <c r="O1006" s="1"/>
+      <c r="P1006" s="1"/>
+      <c r="Q1006" s="1"/>
+      <c r="R1006" s="1"/>
+      <c r="S1006" s="1"/>
+      <c r="T1006" s="1"/>
+      <c r="U1006" s="1"/>
+      <c r="V1006" s="1"/>
+      <c r="W1006" s="1"/>
+      <c r="X1006" s="1"/>
+      <c r="Y1006" s="1"/>
+      <c r="Z1006" s="1"/>
+      <c r="AA1006" s="1"/>
+      <c r="AB1006" s="1"/>
+    </row>
+    <row r="1007" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="1"/>
+      <c r="E1007" s="2"/>
+      <c r="F1007" s="1"/>
+      <c r="G1007" s="1"/>
+      <c r="H1007" s="1"/>
+      <c r="I1007" s="1"/>
+      <c r="J1007" s="1"/>
+      <c r="K1007" s="1"/>
+      <c r="L1007" s="1"/>
+      <c r="M1007" s="1"/>
+      <c r="N1007" s="1"/>
+      <c r="O1007" s="1"/>
+      <c r="P1007" s="1"/>
+      <c r="Q1007" s="1"/>
+      <c r="R1007" s="1"/>
+      <c r="S1007" s="1"/>
+      <c r="T1007" s="1"/>
+      <c r="U1007" s="1"/>
+      <c r="V1007" s="1"/>
+      <c r="W1007" s="1"/>
+      <c r="X1007" s="1"/>
+      <c r="Y1007" s="1"/>
+      <c r="Z1007" s="1"/>
+      <c r="AA1007" s="1"/>
+      <c r="AB1007" s="1"/>
+    </row>
+    <row r="1008" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+      <c r="D1008" s="1"/>
+      <c r="E1008" s="2"/>
+      <c r="F1008" s="1"/>
+      <c r="G1008" s="1"/>
+      <c r="H1008" s="1"/>
+      <c r="I1008" s="1"/>
+      <c r="J1008" s="1"/>
+      <c r="K1008" s="1"/>
+      <c r="L1008" s="1"/>
+      <c r="M1008" s="1"/>
+      <c r="N1008" s="1"/>
+      <c r="O1008" s="1"/>
+      <c r="P1008" s="1"/>
+      <c r="Q1008" s="1"/>
+      <c r="R1008" s="1"/>
+      <c r="S1008" s="1"/>
+      <c r="T1008" s="1"/>
+      <c r="U1008" s="1"/>
+      <c r="V1008" s="1"/>
+      <c r="W1008" s="1"/>
+      <c r="X1008" s="1"/>
+      <c r="Y1008" s="1"/>
+      <c r="Z1008" s="1"/>
+      <c r="AA1008" s="1"/>
+      <c r="AB1008" s="1"/>
+    </row>
+    <row r="1009" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="1"/>
+      <c r="C1009" s="1"/>
+      <c r="D1009" s="1"/>
+      <c r="E1009" s="2"/>
+      <c r="F1009" s="1"/>
+      <c r="G1009" s="1"/>
+      <c r="H1009" s="1"/>
+      <c r="I1009" s="1"/>
+      <c r="J1009" s="1"/>
+      <c r="K1009" s="1"/>
+      <c r="L1009" s="1"/>
+      <c r="M1009" s="1"/>
+      <c r="N1009" s="1"/>
+      <c r="O1009" s="1"/>
+      <c r="P1009" s="1"/>
+      <c r="Q1009" s="1"/>
+      <c r="R1009" s="1"/>
+      <c r="S1009" s="1"/>
+      <c r="T1009" s="1"/>
+      <c r="U1009" s="1"/>
+      <c r="V1009" s="1"/>
+      <c r="W1009" s="1"/>
+      <c r="X1009" s="1"/>
+      <c r="Y1009" s="1"/>
+      <c r="Z1009" s="1"/>
+      <c r="AA1009" s="1"/>
+      <c r="AB1009" s="1"/>
+    </row>
+    <row r="1010" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1010" s="1"/>
+      <c r="B1010" s="1"/>
+      <c r="C1010" s="1"/>
+      <c r="D1010" s="1"/>
+      <c r="E1010" s="2"/>
+      <c r="F1010" s="1"/>
+      <c r="G1010" s="1"/>
+      <c r="H1010" s="1"/>
+      <c r="I1010" s="1"/>
+      <c r="J1010" s="1"/>
+      <c r="K1010" s="1"/>
+      <c r="L1010" s="1"/>
+      <c r="M1010" s="1"/>
+      <c r="N1010" s="1"/>
+      <c r="O1010" s="1"/>
+      <c r="P1010" s="1"/>
+      <c r="Q1010" s="1"/>
+      <c r="R1010" s="1"/>
+      <c r="S1010" s="1"/>
+      <c r="T1010" s="1"/>
+      <c r="U1010" s="1"/>
+      <c r="V1010" s="1"/>
+      <c r="W1010" s="1"/>
+      <c r="X1010" s="1"/>
+      <c r="Y1010" s="1"/>
+      <c r="Z1010" s="1"/>
+      <c r="AA1010" s="1"/>
+      <c r="AB1010" s="1"/>
+    </row>
+    <row r="1011" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1011" s="1"/>
+      <c r="B1011" s="1"/>
+      <c r="C1011" s="1"/>
+      <c r="D1011" s="1"/>
+      <c r="E1011" s="2"/>
+      <c r="F1011" s="1"/>
+      <c r="G1011" s="1"/>
+      <c r="H1011" s="1"/>
+      <c r="I1011" s="1"/>
+      <c r="J1011" s="1"/>
+      <c r="K1011" s="1"/>
+      <c r="L1011" s="1"/>
+      <c r="M1011" s="1"/>
+      <c r="N1011" s="1"/>
+      <c r="O1011" s="1"/>
+      <c r="P1011" s="1"/>
+      <c r="Q1011" s="1"/>
+      <c r="R1011" s="1"/>
+      <c r="S1011" s="1"/>
+      <c r="T1011" s="1"/>
+      <c r="U1011" s="1"/>
+      <c r="V1011" s="1"/>
+      <c r="W1011" s="1"/>
+      <c r="X1011" s="1"/>
+      <c r="Y1011" s="1"/>
+      <c r="Z1011" s="1"/>
+      <c r="AA1011" s="1"/>
+      <c r="AB1011" s="1"/>
+    </row>
+    <row r="1012" spans="1:28" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A1012" s="1"/>
+      <c r="B1012" s="1"/>
+      <c r="C1012" s="1"/>
+      <c r="D1012" s="1"/>
+      <c r="E1012" s="2"/>
+      <c r="F1012" s="1"/>
+      <c r="G1012" s="1"/>
+      <c r="H1012" s="1"/>
+      <c r="I1012" s="1"/>
+      <c r="J1012" s="1"/>
+      <c r="K1012" s="1"/>
+      <c r="L1012" s="1"/>
+      <c r="M1012" s="1"/>
+      <c r="N1012" s="1"/>
+      <c r="O1012" s="1"/>
+      <c r="P1012" s="1"/>
+      <c r="Q1012" s="1"/>
+      <c r="R1012" s="1"/>
+      <c r="S1012" s="1"/>
+      <c r="T1012" s="1"/>
+      <c r="U1012" s="1"/>
+      <c r="V1012" s="1"/>
+      <c r="W1012" s="1"/>
+      <c r="X1012" s="1"/>
+      <c r="Y1012" s="1"/>
+      <c r="Z1012" s="1"/>
+      <c r="AA1012" s="1"/>
+      <c r="AB1012" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="I2:I16 I18:I1002" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I22 I24:I1012" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>